<commit_message>
interfacce, diario,doc, gantt e requisiti
</commit_message>
<xml_diff>
--- a/Progettazione/Analisi/Requisiti.xlsx
+++ b/Progettazione/Analisi/Requisiti.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="70">
   <si>
     <t>ID</t>
   </si>
@@ -104,9 +104,6 @@
     <t>Conferma registrazione</t>
   </si>
   <si>
-    <t>In caso di password persa l'A. può creare una password momentanea</t>
-  </si>
-  <si>
     <t>Dopo la conferma di registrazione il docente può creare una password</t>
   </si>
   <si>
@@ -161,9 +158,6 @@
     <t>Può confermare la registrazione</t>
   </si>
   <si>
-    <t>Può modificare la password dei docenti in caso di dimenticanza</t>
-  </si>
-  <si>
     <t>Effettua il login</t>
   </si>
   <si>
@@ -237,6 +231,9 @@
   </si>
   <si>
     <t>accesso a "Visioni particolari" a tutti</t>
+  </si>
+  <si>
+    <t>insegnano le materie alle classi a dipendenza del corso della classe</t>
   </si>
 </sst>
 </file>
@@ -246,7 +243,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -258,13 +255,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -331,7 +321,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -356,9 +346,6 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -652,10 +639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:D131"/>
+  <dimension ref="C1:D130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B88" workbookViewId="0">
-      <selection activeCell="D131" sqref="D131"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -721,19 +708,19 @@
     <row r="10" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C10" s="10"/>
       <c r="D10" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C11" s="10"/>
       <c r="D11" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C12" s="9"/>
       <c r="D12" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -877,7 +864,7 @@
     <row r="35" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C35" s="9"/>
       <c r="D35" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -938,133 +925,133 @@
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C46" s="9"/>
-      <c r="D46" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="47" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C46" s="1"/>
+    </row>
+    <row r="47" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C47" s="1"/>
     </row>
     <row r="48" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C48" s="1"/>
+      <c r="C48" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="49" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C49" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>23</v>
+        <v>2</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="50" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C50" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>12</v>
+        <v>3</v>
+      </c>
+      <c r="D50" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C51" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D51" s="3">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="52" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C52" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D52" s="6" t="s">
-        <v>7</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D52" s="3"/>
     </row>
     <row r="53" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C53" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D53" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="54" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C54" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D54" s="7" t="s">
-        <v>8</v>
+      <c r="C54" s="9"/>
+      <c r="D54" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="55" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C55" s="9"/>
       <c r="D55" s="3" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
     </row>
     <row r="56" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C56" s="9"/>
       <c r="D56" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="57" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C57" s="9"/>
-      <c r="D57" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="58" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="59" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="57" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="59" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C59" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
     <row r="60" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C60" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D60" s="7" t="s">
-        <v>29</v>
+        <v>2</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="61" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C61" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>28</v>
+        <v>3</v>
+      </c>
+      <c r="D61" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C62" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D62" s="3">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="63" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C63" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D63" s="6" t="s">
-        <v>7</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D63" s="3"/>
     </row>
     <row r="64" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C64" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D64" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="D64" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="65" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C65" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D65" s="7" t="s">
-        <v>8</v>
+      <c r="C65" s="9"/>
+      <c r="D65" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="66" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C66" s="9"/>
-      <c r="D66" s="3" t="s">
+      <c r="C66" s="10"/>
+      <c r="D66" s="4" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1075,96 +1062,96 @@
       </c>
     </row>
     <row r="68" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C68" s="10"/>
-      <c r="D68" s="4" t="s">
-        <v>44</v>
+      <c r="C68" s="9"/>
+      <c r="D68" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="69" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C69" s="9"/>
-      <c r="D69" s="11" t="s">
-        <v>45</v>
+      <c r="D69" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="70" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C70" s="9"/>
       <c r="D70" s="3" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
     </row>
     <row r="71" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C71" s="9"/>
       <c r="D71" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="72" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C72" s="9"/>
-      <c r="D72" s="3" t="s">
-        <v>53</v>
-      </c>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="72" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C72" s="1"/>
     </row>
     <row r="73" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C73" s="9"/>
-      <c r="D73" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="74" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C74" s="1"/>
+      <c r="C73" s="1"/>
+    </row>
+    <row r="74" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C74" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D74" s="7" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="75" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C75" s="1"/>
+      <c r="C75" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="76" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C76" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D76" s="7" t="s">
-        <v>30</v>
+        <v>3</v>
+      </c>
+      <c r="D76" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C77" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>33</v>
+        <v>6</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="78" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C78" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D78" s="3">
-        <v>1</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D78" s="3"/>
     </row>
     <row r="79" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C79" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D79" s="6" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="D79" s="7" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="80" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C80" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D80" s="3"/>
+      <c r="C80" s="10"/>
+      <c r="D80" s="4" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="81" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C81" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D81" s="7" t="s">
-        <v>8</v>
+      <c r="C81" s="9"/>
+      <c r="D81" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="82" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C82" s="10"/>
-      <c r="D82" s="4" t="s">
+      <c r="C82" s="9"/>
+      <c r="D82" s="3" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1181,223 +1168,223 @@
       </c>
     </row>
     <row r="85" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C85" s="9"/>
+      <c r="C85" s="10"/>
       <c r="D85" s="3" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="86" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C86" s="9"/>
       <c r="D86" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="87" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C87" s="10"/>
-      <c r="D87" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="88" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C88" s="9"/>
-      <c r="D88" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="89" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C89" s="10"/>
-      <c r="D89" s="4"/>
-    </row>
-    <row r="90" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="91" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+      <c r="D87" s="4"/>
+    </row>
+    <row r="88" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="89" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="90" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C90" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D90" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="91" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C91" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
     <row r="92" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C92" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D92" s="7" t="s">
-        <v>31</v>
+        <v>3</v>
+      </c>
+      <c r="D92" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C93" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D93" s="3" t="s">
-        <v>36</v>
+        <v>6</v>
+      </c>
+      <c r="D93" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="94" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C94" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D94" s="3">
-        <v>1</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D94" s="3"/>
     </row>
     <row r="95" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C95" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D95" s="6" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="D95" s="7" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="96" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C96" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D96" s="3"/>
+      <c r="C96" s="10"/>
+      <c r="D96" s="4" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="97" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C97" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D97" s="7" t="s">
-        <v>8</v>
+      <c r="C97" s="10"/>
+      <c r="D97" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="98" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C98" s="10"/>
-      <c r="D98" s="4" t="s">
-        <v>55</v>
+      <c r="D98" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="99" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C99" s="10"/>
       <c r="D99" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="100" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C100" s="9"/>
+      <c r="D100" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="100" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C100" s="10"/>
-      <c r="D100" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="101" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C101" s="9"/>
-      <c r="D101" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="103" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="102" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="103" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C103" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D103" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
     <row r="104" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C104" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D104" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D104" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="105" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C105" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D105" s="3" t="s">
-        <v>38</v>
+        <v>3</v>
+      </c>
+      <c r="D105" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="106" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C106" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D106" s="3">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="D106" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="107" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C107" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D107" s="6" t="s">
-        <v>7</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D107" s="3"/>
     </row>
     <row r="108" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C108" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D108" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="D108" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="109" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C109" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D109" s="7" t="s">
-        <v>8</v>
+      <c r="C109" s="9"/>
+      <c r="D109" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="110" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C110" s="9"/>
-      <c r="D110" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="111" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C111" s="9"/>
-      <c r="D111" s="3"/>
-    </row>
-    <row r="113" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+      <c r="D110" s="3"/>
+    </row>
+    <row r="112" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="113" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C113" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D113" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
     <row r="114" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C114" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D114" s="7" t="s">
-        <v>58</v>
+        <v>2</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="115" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C115" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D115" s="3" t="s">
-        <v>59</v>
+        <v>3</v>
+      </c>
+      <c r="D115" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="116" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C116" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D116" s="3">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="D116" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="117" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C117" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D117" s="6" t="s">
-        <v>7</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D117" s="3"/>
     </row>
     <row r="118" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C118" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D118" s="3"/>
-    </row>
-    <row r="119" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C119" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D119" s="7" t="s">
+      <c r="D118" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="120" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C119" s="13"/>
+      <c r="D119" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="120" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C120" s="14"/>
-      <c r="D120" s="12" t="s">
-        <v>60</v>
-      </c>
+      <c r="D120" s="12"/>
     </row>
     <row r="121" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C121" s="15"/>
-      <c r="D121" s="13"/>
+      <c r="C121" s="9"/>
+      <c r="D121" s="3" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="122" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C122" s="9"/>
       <c r="D122" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="123" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1409,19 +1396,19 @@
     <row r="124" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C124" s="9"/>
       <c r="D124" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="125" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C125" s="9"/>
       <c r="D125" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="126" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C126" s="9"/>
       <c r="D126" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="127" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1433,31 +1420,25 @@
     <row r="128" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C128" s="9"/>
       <c r="D128" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="129" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C129" s="9"/>
       <c r="D129" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="130" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C130" s="9"/>
       <c r="D130" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="131" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C131" s="9"/>
-      <c r="D131" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="D120:D121"/>
-    <mergeCell ref="C120:C121"/>
+    <mergeCell ref="D119:D120"/>
+    <mergeCell ref="C119:C120"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
aggiunta presentazione fatta e modifica consuntivo+scorsa settimana
</commit_message>
<xml_diff>
--- a/Progettazione/Analisi/Requisiti.xlsx
+++ b/Progettazione/Analisi/Requisiti.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MPT\Progettazione\Analisi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MPT\Progettazione\Analisi\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="74">
   <si>
     <t>ID</t>
   </si>
@@ -92,9 +92,6 @@
     <t>la conferma della registrazione deve avvenire entro 3 giorni</t>
   </si>
   <si>
-    <t>La registrazione deve essere confermata dall'A. prima di effettuare il login</t>
-  </si>
-  <si>
     <t>REQ-004</t>
   </si>
   <si>
@@ -104,9 +101,6 @@
     <t>Conferma registrazione</t>
   </si>
   <si>
-    <t>Dopo la conferma di registrazione il docente può creare una password</t>
-  </si>
-  <si>
     <t>Amministratore</t>
   </si>
   <si>
@@ -155,9 +149,6 @@
     <t>Può creare o eliminare i responsabili</t>
   </si>
   <si>
-    <t>Può confermare la registrazione</t>
-  </si>
-  <si>
     <t>Effettua il login</t>
   </si>
   <si>
@@ -234,6 +225,27 @@
   </si>
   <si>
     <t>insegnano le materie alle classi a dipendenza del corso della classe</t>
+  </si>
+  <si>
+    <t>La registrazione deve essere confermata da gestore email prima di effettuare il login</t>
+  </si>
+  <si>
+    <t>Dopo la conferma di registrazione il docente può creare una nuova password</t>
+  </si>
+  <si>
+    <t>l'email per il login deve essere fatto con l'email scolastica</t>
+  </si>
+  <si>
+    <t>C'è un gestore delle email</t>
+  </si>
+  <si>
+    <t>Può aggiungere o eliminare classi nel DB</t>
+  </si>
+  <si>
+    <t>Può aggiungere o eliminare corsi nel DB</t>
+  </si>
+  <si>
+    <t>tutti hanno accesso alla pagina di registrazione</t>
   </si>
 </sst>
 </file>
@@ -260,12 +272,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -321,7 +339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -347,6 +365,9 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -358,6 +379,26 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -639,16 +680,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:D130"/>
+  <dimension ref="C1:D134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="D99" sqref="D99"/>
+    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
+      <selection activeCell="D125" sqref="D125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="13.109375" customWidth="1"/>
-    <col min="4" max="4" width="62.21875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="62.88671875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -708,19 +749,19 @@
     <row r="10" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C10" s="10"/>
       <c r="D10" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C11" s="10"/>
       <c r="D11" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C12" s="9"/>
       <c r="D12" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -816,7 +857,7 @@
         <v>2</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -855,16 +896,16 @@
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C34" s="9"/>
       <c r="D34" s="4" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C35" s="9"/>
       <c r="D35" s="3" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -922,523 +963,548 @@
     <row r="45" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C45" s="10"/>
       <c r="D45" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="46" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C46" s="1"/>
-    </row>
-    <row r="47" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C47" s="1"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C46" s="10"/>
+      <c r="D46" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="47" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C47" s="16"/>
+      <c r="D47" s="17"/>
     </row>
     <row r="48" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C48" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>23</v>
-      </c>
+      <c r="C48" s="1"/>
     </row>
     <row r="49" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C49" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>12</v>
+        <v>0</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="50" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C50" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D50" s="3">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="51" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C51" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>7</v>
+        <v>3</v>
+      </c>
+      <c r="D51" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C52" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D52" s="3"/>
+        <v>6</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="53" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C53" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D53" s="3"/>
+    </row>
+    <row r="54" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C54" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D53" s="7" t="s">
+      <c r="D54" s="7" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="54" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C54" s="9"/>
-      <c r="D54" s="3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="55" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C55" s="9"/>
       <c r="D55" s="3" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="56" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C56" s="9"/>
       <c r="D56" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="57" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C57" s="9"/>
+      <c r="D57" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="58" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C58" s="9"/>
+      <c r="D58" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="57" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="58" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="59" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C59" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D59" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="60" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C60" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
+    <row r="59" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="61" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C61" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D61" s="3">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="62" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C62" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D62" s="6" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="63" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C63" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D63" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="D63" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="64" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C64" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C65" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D65" s="3"/>
+    </row>
+    <row r="66" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C66" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D64" s="7" t="s">
+      <c r="D66" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C65" s="9"/>
-      <c r="D65" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="66" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C66" s="10"/>
-      <c r="D66" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
     <row r="67" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C67" s="10"/>
-      <c r="D67" s="4" t="s">
-        <v>43</v>
+      <c r="C67" s="9"/>
+      <c r="D67" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="68" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C68" s="9"/>
-      <c r="D68" s="3" t="s">
+      <c r="C68" s="10"/>
+      <c r="D68" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="69" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C69" s="9"/>
       <c r="D69" s="3" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
     </row>
     <row r="70" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C70" s="9"/>
       <c r="D70" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="71" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C71" s="9"/>
       <c r="D71" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="72" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C72" s="1"/>
-    </row>
-    <row r="73" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="72" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C72" s="9"/>
+      <c r="D72" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="73" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C73" s="1"/>
     </row>
     <row r="74" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C74" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D74" s="7" t="s">
-        <v>29</v>
-      </c>
+      <c r="C74" s="1"/>
     </row>
     <row r="75" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C75" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>32</v>
+        <v>0</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="76" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C76" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D76" s="3">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="77" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C77" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D77" s="6" t="s">
-        <v>7</v>
+        <v>3</v>
+      </c>
+      <c r="D77" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C78" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D78" s="3"/>
+        <v>6</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="79" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C79" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D79" s="3"/>
+    </row>
+    <row r="80" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C80" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D79" s="7" t="s">
+      <c r="D80" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="80" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C80" s="10"/>
-      <c r="D80" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="81" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C81" s="9"/>
-      <c r="D81" s="3" t="s">
-        <v>46</v>
+    <row r="81" spans="3:4" s="20" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C81" s="18"/>
+      <c r="D81" s="19" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="82" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C82" s="9"/>
       <c r="D82" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="83" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C83" s="9"/>
       <c r="D83" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="84" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C84" s="9"/>
-      <c r="D84" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="84" spans="3:4" s="20" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C84" s="21"/>
+      <c r="D84" s="22" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="85" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C85" s="10"/>
+      <c r="C85" s="9"/>
       <c r="D85" s="3" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="86" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C86" s="9"/>
       <c r="D86" s="3" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
     </row>
     <row r="87" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C87" s="10"/>
-      <c r="D87" s="4"/>
-    </row>
-    <row r="88" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="89" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="90" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C90" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D90" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="91" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C91" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D91" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="92" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C92" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D92" s="3">
-        <v>1</v>
-      </c>
-    </row>
+      <c r="C87" s="9"/>
+      <c r="D87" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="88" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C88" s="10"/>
+      <c r="D88" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="89" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C89" s="9"/>
+      <c r="D89" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="90" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C90" s="10"/>
+      <c r="D90" s="4"/>
+    </row>
+    <row r="91" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="92" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="93" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C93" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D93" s="6" t="s">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="D93" s="7" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="94" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C94" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D94" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="95" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C95" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D95" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C96" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D96" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="97" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C97" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D97" s="3"/>
+    </row>
+    <row r="98" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C98" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D95" s="7" t="s">
+      <c r="D98" s="7" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="96" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C96" s="10"/>
-      <c r="D96" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="97" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C97" s="10"/>
-      <c r="D97" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="98" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C98" s="10"/>
-      <c r="D98" s="3" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="99" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C99" s="10"/>
-      <c r="D99" s="3" t="s">
-        <v>69</v>
+      <c r="D99" s="4" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="100" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C100" s="9"/>
+      <c r="C100" s="10"/>
       <c r="D100" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="102" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="101" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C101" s="10"/>
+      <c r="D101" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="102" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C102" s="10"/>
+      <c r="D102" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
     <row r="103" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C103" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D103" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="104" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C104" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D104" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="105" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C105" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D105" s="3">
-        <v>1</v>
-      </c>
-    </row>
+      <c r="C103" s="9"/>
+      <c r="D103" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="105" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="106" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C106" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D106" s="6" t="s">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="D106" s="7" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="107" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C107" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D107" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="108" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C108" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D108" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C109" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D109" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="110" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C110" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D110" s="3"/>
+    </row>
+    <row r="111" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C111" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D108" s="7" t="s">
+      <c r="D111" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="109" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C109" s="9"/>
-      <c r="D109" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="110" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C110" s="9"/>
-      <c r="D110" s="3"/>
-    </row>
-    <row r="112" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="112" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C112" s="9"/>
+      <c r="D112" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
     <row r="113" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C113" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D113" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="114" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C114" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D114" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="115" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C115" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D115" s="3">
-        <v>1</v>
-      </c>
-    </row>
+      <c r="C113" s="9"/>
+      <c r="D113" s="3"/>
+    </row>
+    <row r="115" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="116" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C116" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D116" s="6" t="s">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="D116" s="7" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="117" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C117" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D117" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="118" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C118" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D118" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C119" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D119" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="120" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C120" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D120" s="3"/>
+    </row>
+    <row r="121" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C121" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D118" s="7" t="s">
+      <c r="D121" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="119" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C119" s="13"/>
-      <c r="D119" s="11" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="120" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C120" s="14"/>
-      <c r="D120" s="12"/>
-    </row>
-    <row r="121" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C121" s="9"/>
-      <c r="D121" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="122" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C122" s="9"/>
-      <c r="D122" s="3" t="s">
-        <v>60</v>
+    <row r="122" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C122" s="14"/>
+      <c r="D122" s="12" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="123" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C123" s="9"/>
-      <c r="D123" s="3" t="s">
-        <v>62</v>
-      </c>
+      <c r="C123" s="15"/>
+      <c r="D123" s="13"/>
     </row>
     <row r="124" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C124" s="9"/>
-      <c r="D124" s="3" t="s">
-        <v>61</v>
+      <c r="C124" s="11"/>
+      <c r="D124" s="23" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="125" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C125" s="9"/>
       <c r="D125" s="3" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="126" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C126" s="9"/>
       <c r="D126" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="127" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C127" s="9"/>
       <c r="D127" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="128" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C128" s="9"/>
       <c r="D128" s="3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="129" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C129" s="9"/>
       <c r="D129" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="130" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C130" s="9"/>
       <c r="D130" s="3" t="s">
-        <v>68</v>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="131" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C131" s="9"/>
+      <c r="D131" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="132" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C132" s="9"/>
+      <c r="D132" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="133" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C133" s="9"/>
+      <c r="D133" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="134" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C134" s="9"/>
+      <c r="D134" s="3" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="D119:D120"/>
-    <mergeCell ref="C119:C120"/>
+    <mergeCell ref="D122:D123"/>
+    <mergeCell ref="C122:C123"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
aggiunta captcha, documentazione, diario, inserimento commenti nei vari file
</commit_message>
<xml_diff>
--- a/Progettazione/Analisi/Requisiti.xlsx
+++ b/Progettazione/Analisi/Requisiti.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MPT\Progettazione\Analisi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MPT\Progettazione\Analisi\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="74">
   <si>
     <t>ID</t>
   </si>
@@ -197,9 +197,6 @@
     <t>tutti hanno accesso alla pagina login</t>
   </si>
   <si>
-    <t>admin ha accesso alla sua pagina amministrazione</t>
-  </si>
-  <si>
     <t>accesso a "Menu Principale AIT" a tutti</t>
   </si>
   <si>
@@ -246,6 +243,9 @@
   </si>
   <si>
     <t>tutti hanno accesso alla pagina di registrazione</t>
+  </si>
+  <si>
+    <t>admin ha accesso alla sua pagina amministrazione e a tutte le altre pagine</t>
   </si>
 </sst>
 </file>
@@ -368,18 +368,6 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -399,6 +387,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -682,8 +682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:D134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="D125" sqref="D125"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="D85" sqref="D85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -899,13 +899,13 @@
     <row r="34" spans="3:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C34" s="9"/>
       <c r="D34" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C35" s="9"/>
       <c r="D35" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -969,12 +969,12 @@
     <row r="46" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C46" s="10"/>
       <c r="D46" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="47" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C47" s="16"/>
-      <c r="D47" s="17"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="13"/>
     </row>
     <row r="48" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C48" s="1"/>
@@ -1040,7 +1040,7 @@
     <row r="57" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C57" s="9"/>
       <c r="D57" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="58" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1185,9 +1185,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="81" spans="3:4" s="20" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C81" s="18"/>
-      <c r="D81" s="19" t="s">
+    <row r="81" spans="3:4" s="16" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C81" s="14"/>
+      <c r="D81" s="15" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1203,9 +1203,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="84" spans="3:4" s="20" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C84" s="21"/>
-      <c r="D84" s="22" t="s">
+    <row r="84" spans="3:4" s="16" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C84" s="17"/>
+      <c r="D84" s="18" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1218,13 +1218,13 @@
     <row r="86" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C86" s="9"/>
       <c r="D86" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="87" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C87" s="9"/>
       <c r="D87" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="88" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1241,7 +1241,9 @@
     </row>
     <row r="90" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C90" s="10"/>
-      <c r="D90" s="4"/>
+      <c r="D90" s="4" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="91" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="92" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1312,7 +1314,7 @@
     <row r="102" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C102" s="10"/>
       <c r="D102" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="103" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1426,19 +1428,19 @@
       </c>
     </row>
     <row r="122" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C122" s="14"/>
-      <c r="D122" s="12" t="s">
+      <c r="C122" s="22"/>
+      <c r="D122" s="20" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="123" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C123" s="15"/>
-      <c r="D123" s="13"/>
+      <c r="C123" s="23"/>
+      <c r="D123" s="21"/>
     </row>
     <row r="124" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C124" s="11"/>
-      <c r="D124" s="23" t="s">
-        <v>73</v>
+      <c r="D124" s="19" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="125" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1450,55 +1452,55 @@
     <row r="126" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C126" s="9"/>
       <c r="D126" s="3" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
     </row>
     <row r="127" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C127" s="9"/>
       <c r="D127" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="128" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C128" s="9"/>
       <c r="D128" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="129" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C129" s="9"/>
       <c r="D129" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="130" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C130" s="9"/>
       <c r="D130" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="131" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C131" s="9"/>
       <c r="D131" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="132" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C132" s="9"/>
       <c r="D132" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="133" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C133" s="9"/>
       <c r="D133" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="134" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C134" s="9"/>
       <c r="D134" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Eliminazione della cartella altro, aggiunti commenti ai codici, modiche della doc, modifica dei file di progettazione
</commit_message>
<xml_diff>
--- a/Progettazione/Analisi/Requisiti.xlsx
+++ b/Progettazione/Analisi/Requisiti.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MPT\Progettazione\Analisi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MPT\Progettazione\Analisi\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="70">
   <si>
     <t>ID</t>
   </si>
@@ -152,9 +152,6 @@
     <t>Effettua il login</t>
   </si>
   <si>
-    <t>Può inserire,cancellare,modificare dati, ecc.. Nei campi</t>
-  </si>
-  <si>
     <t>Deve poter pianificare i docenti</t>
   </si>
   <si>
@@ -164,9 +161,6 @@
     <t>Non può cancellare eventuali altri responsabili</t>
   </si>
   <si>
-    <t>Può aggiungere o eliminare materie nel DB</t>
-  </si>
-  <si>
     <t>Effettuano il login</t>
   </si>
   <si>
@@ -179,51 +173,21 @@
     <t xml:space="preserve">Inseriscono le ore delle proprie lezioni </t>
   </si>
   <si>
-    <t xml:space="preserve">Ha tutti i permessi e i requisiti che ha un docente </t>
-  </si>
-  <si>
-    <t>Può aggiungere o eliminare dati nel DB(materie,classi,…) tramite il sito web</t>
-  </si>
-  <si>
     <t>REQ-010</t>
   </si>
   <si>
     <t>Permessi</t>
   </si>
   <si>
-    <t>l'admin ha accesso a tutte le pagine web(pagine personali del docente non comprese)</t>
-  </si>
-  <si>
     <t>tutti hanno accesso alla pagina login</t>
   </si>
   <si>
-    <t>accesso a "Menu Principale AIT" a tutti</t>
-  </si>
-  <si>
     <t>accesso a "Gestione Accessi Docenti" solo a R</t>
   </si>
   <si>
-    <t>accesso a "Inserimento ore AIT" solo a docenti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">accesso a "Pianificazione Docenti MPT (Responsabile)" solo a R </t>
-  </si>
-  <si>
     <t>accesso a "Visione pianificazione… (Responsabile)" solo a R</t>
   </si>
   <si>
-    <t>accesso a "VIsione pianificazione… (docente)" solo a docente</t>
-  </si>
-  <si>
-    <t>accesso a "Visione pianoficazione completa…" solo a R</t>
-  </si>
-  <si>
-    <t>accesso a "Visioni particolari" a tutti</t>
-  </si>
-  <si>
-    <t>insegnano le materie alle classi a dipendenza del corso della classe</t>
-  </si>
-  <si>
     <t>La registrazione deve essere confermata da gestore email prima di effettuare il login</t>
   </si>
   <si>
@@ -236,16 +200,40 @@
     <t>C'è un gestore delle email</t>
   </si>
   <si>
-    <t>Può aggiungere o eliminare classi nel DB</t>
-  </si>
-  <si>
-    <t>Può aggiungere o eliminare corsi nel DB</t>
-  </si>
-  <si>
     <t>tutti hanno accesso alla pagina di registrazione</t>
   </si>
   <si>
-    <t>admin ha accesso alla sua pagina amministrazione e a tutte le altre pagine</t>
+    <t>tutti hanno accesso alla pagina di password dimenticata</t>
+  </si>
+  <si>
+    <t>accesso a "Menu Principale AIT" a tutti quelli che hanno effettuato il login</t>
+  </si>
+  <si>
+    <t>accesso a "Inserimento ore AIT" solo agli user di tipo docente</t>
+  </si>
+  <si>
+    <t>accesso a "Visione pianificazione… (docente)" solo agli user di tipo docente</t>
+  </si>
+  <si>
+    <t>accesso a "Visione pianificazione completa…" a tutti quelli loggati</t>
+  </si>
+  <si>
+    <t>accesso a "Visioni particolari" a tutti quelli che hanno effettuato il login</t>
+  </si>
+  <si>
+    <t>l'admin ha accesso a tutte le pagine web</t>
+  </si>
+  <si>
+    <t>accesso a "Pianificazione Docenti MPT (Responsabile)" solo a R</t>
+  </si>
+  <si>
+    <t>Ha solo accesso alle pagine del responsabile</t>
+  </si>
+  <si>
+    <t>Ha accesso solo alle pagine del docente</t>
+  </si>
+  <si>
+    <t>Può aggiungere o eliminare dati nel DB(materie,classi,corso,...) tramite il sito web</t>
   </si>
 </sst>
 </file>
@@ -272,18 +260,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -339,7 +321,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -374,31 +356,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -680,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:D134"/>
+  <dimension ref="C1:D125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="D85" sqref="D85"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -764,749 +740,730 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C13" s="1"/>
       <c r="D13" s="5"/>
     </row>
     <row r="14" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C14" s="1"/>
+      <c r="C14" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="15" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C15" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>11</v>
+        <v>2</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C16" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>17</v>
+        <v>3</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C17" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D17" s="3">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C18" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>7</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D18" s="3"/>
     </row>
     <row r="19" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C19" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="20" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>8</v>
+      <c r="C20" s="10"/>
+      <c r="D20" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C21" s="10"/>
-      <c r="D21" s="4" t="s">
-        <v>18</v>
+      <c r="C21" s="9"/>
+      <c r="D21" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C22" s="9"/>
       <c r="D22" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C23" s="9"/>
-      <c r="D23" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="D23" s="3"/>
     </row>
     <row r="24" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C24" s="9"/>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C25" s="9"/>
-      <c r="D25" s="3"/>
-    </row>
-    <row r="26" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
     <row r="27" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C27" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>15</v>
+        <v>2</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C28" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>24</v>
+        <v>3</v>
+      </c>
+      <c r="D28" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C29" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D29" s="3">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C30" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>7</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D30" s="3"/>
     </row>
     <row r="31" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C31" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="32" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C32" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C33" s="10"/>
-      <c r="D33" s="3" t="s">
+      <c r="C32" s="10"/>
+      <c r="D32" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="3:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C33" s="9"/>
+      <c r="D33" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C34" s="9"/>
-      <c r="D34" s="4" t="s">
-        <v>66</v>
+      <c r="D34" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C35" s="9"/>
-      <c r="D35" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="36" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C36" s="9"/>
-      <c r="D36" s="3"/>
-    </row>
-    <row r="37" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="38" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="37" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C37" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C38" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="39" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C39" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>15</v>
+        <v>3</v>
+      </c>
+      <c r="D39" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C40" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>16</v>
+        <v>6</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C41" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D41" s="3">
-        <v>1</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D41" s="3"/>
     </row>
     <row r="42" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C42" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C43" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D43" s="3"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="44" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C44" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>8</v>
+      <c r="C44" s="10"/>
+      <c r="D44" s="4" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C45" s="10"/>
-      <c r="D45" s="4" t="s">
-        <v>23</v>
-      </c>
+      <c r="C45" s="12"/>
+      <c r="D45" s="13"/>
     </row>
     <row r="46" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C46" s="10"/>
-      <c r="D46" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="47" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C47" s="12"/>
-      <c r="D47" s="13"/>
+      <c r="C46" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C47" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="48" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C48" s="1"/>
+      <c r="C48" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D48" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="49" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C49" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>22</v>
+        <v>6</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C50" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>12</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D50" s="3"/>
     </row>
     <row r="51" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C51" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D51" s="3">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="52" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C52" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D52" s="6" t="s">
-        <v>7</v>
+      <c r="C52" s="9"/>
+      <c r="D52" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="53" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C53" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D53" s="3"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="54" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C54" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D54" s="7" t="s">
-        <v>8</v>
+      <c r="C54" s="9"/>
+      <c r="D54" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="55" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C55" s="9"/>
       <c r="D55" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="56" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C56" s="9"/>
-      <c r="D56" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="57" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C57" s="9"/>
-      <c r="D57" s="3" t="s">
-        <v>69</v>
+      <c r="C57" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="58" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C58" s="9"/>
+      <c r="C58" s="8" t="s">
+        <v>2</v>
+      </c>
       <c r="D58" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="59" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="60" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="59" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C59" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D59" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C60" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="61" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C61" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D61" s="7" t="s">
-        <v>26</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D61" s="3"/>
     </row>
     <row r="62" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C62" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>25</v>
+        <v>4</v>
+      </c>
+      <c r="D62" s="7" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="63" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C63" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D63" s="3">
-        <v>1</v>
+      <c r="C63" s="9"/>
+      <c r="D63" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="64" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C64" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D64" s="6" t="s">
-        <v>7</v>
+      <c r="C64" s="10"/>
+      <c r="D64" s="4" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="65" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C65" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D65" s="3"/>
+      <c r="C65" s="9"/>
+      <c r="D65" s="3" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="66" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C66" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D66" s="7" t="s">
-        <v>8</v>
+      <c r="C66" s="9"/>
+      <c r="D66" s="20" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="67" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C67" s="9"/>
-      <c r="D67" s="3" t="s">
-        <v>39</v>
-      </c>
+      <c r="D67" s="21"/>
     </row>
     <row r="68" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C68" s="10"/>
-      <c r="D68" s="4" t="s">
-        <v>40</v>
+      <c r="C68" s="9"/>
+      <c r="D68" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="69" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C69" s="9"/>
       <c r="D69" s="3" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
     <row r="70" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C70" s="9"/>
       <c r="D70" s="3" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
     </row>
     <row r="71" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C71" s="9"/>
-      <c r="D71" s="3" t="s">
-        <v>48</v>
-      </c>
+      <c r="C71" s="1"/>
     </row>
     <row r="72" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C72" s="9"/>
-      <c r="D72" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="73" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C73" s="1"/>
+      <c r="C72" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D72" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="73" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C73" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="74" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C74" s="1"/>
+      <c r="C74" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D74" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="75" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C75" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D75" s="7" t="s">
-        <v>27</v>
+        <v>6</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="76" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C76" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>30</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D76" s="3"/>
     </row>
     <row r="77" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C77" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D77" s="3">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="D77" s="7" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="78" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C78" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D78" s="6" t="s">
-        <v>7</v>
+      <c r="C78" s="9"/>
+      <c r="D78" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="79" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C79" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D79" s="3"/>
+      <c r="C79" s="9"/>
+      <c r="D79" s="3" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="80" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C80" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D80" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="81" spans="3:4" s="16" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C81" s="14"/>
-      <c r="D81" s="15" t="s">
-        <v>42</v>
+      <c r="C80" s="9"/>
+      <c r="D80" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="81" spans="3:4" s="18" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C81" s="16"/>
+      <c r="D81" s="17" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="82" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C82" s="9"/>
       <c r="D82" s="3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="83" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C83" s="9"/>
       <c r="D83" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="84" spans="3:4" s="16" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C84" s="17"/>
-      <c r="D84" s="18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="84" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C84" s="9"/>
+      <c r="D84" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="85" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C85" s="10"/>
+      <c r="D85" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="86" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="87" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C87" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D87" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="88" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C88" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="89" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C89" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D89" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C90" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D90" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="91" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C91" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D91" s="3"/>
+    </row>
+    <row r="92" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C92" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D92" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="93" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C93" s="10"/>
+      <c r="D93" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="94" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C94" s="10"/>
+      <c r="D94" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="85" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C85" s="9"/>
-      <c r="D85" s="3" t="s">
+    <row r="95" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C95" s="10"/>
+      <c r="D95" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="96" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C96" s="10"/>
+      <c r="D96" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="86" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C86" s="9"/>
-      <c r="D86" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="87" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C87" s="9"/>
-      <c r="D87" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="88" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C88" s="10"/>
-      <c r="D88" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="89" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C89" s="9"/>
-      <c r="D89" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="90" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C90" s="10"/>
-      <c r="D90" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="91" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="92" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="93" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C93" s="8" t="s">
+    <row r="97" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C97" s="9"/>
+      <c r="D97" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="98" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="99" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C99" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D93" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="94" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C94" s="8" t="s">
+      <c r="D99" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="100" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C100" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D94" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="95" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C95" s="8" t="s">
+      <c r="D100" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="101" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C101" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D95" s="3">
+      <c r="D101" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C96" s="8" t="s">
+    <row r="102" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C102" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D96" s="6" t="s">
+      <c r="D102" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="97" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C97" s="8" t="s">
+    <row r="103" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C103" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D97" s="3"/>
-    </row>
-    <row r="98" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C98" s="8" t="s">
+      <c r="D103" s="3"/>
+    </row>
+    <row r="104" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C104" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D98" s="7" t="s">
+      <c r="D104" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="99" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C99" s="10"/>
-      <c r="D99" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="100" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C100" s="10"/>
-      <c r="D100" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="101" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C101" s="10"/>
-      <c r="D101" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="102" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C102" s="10"/>
-      <c r="D102" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="103" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C103" s="9"/>
-      <c r="D103" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="105" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="105" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C105" s="9"/>
+      <c r="D105" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
     <row r="106" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C106" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D106" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="107" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C107" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D107" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
+      <c r="C106" s="9"/>
+      <c r="D106" s="3"/>
+    </row>
+    <row r="107" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="108" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C108" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D108" s="3">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D108" s="7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="109" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C109" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D109" s="6" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="110" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C110" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D110" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="D110" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="111" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C111" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D111" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="112" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C112" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D112" s="3"/>
+    </row>
+    <row r="113" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C113" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D111" s="7" t="s">
+      <c r="D113" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="112" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C112" s="9"/>
-      <c r="D112" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="113" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C113" s="9"/>
-      <c r="D113" s="3"/>
-    </row>
-    <row r="115" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="114" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C114" s="19"/>
+      <c r="D114" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="115" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C115" s="11"/>
+      <c r="D115" s="14" t="s">
+        <v>58</v>
+      </c>
+    </row>
     <row r="116" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C116" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D116" s="7" t="s">
+      <c r="C116" s="15"/>
+      <c r="D116" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="117" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C117" s="9"/>
+      <c r="D117" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="118" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C118" s="9"/>
+      <c r="D118" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="119" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C119" s="9"/>
+      <c r="D119" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="120" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C120" s="9"/>
+      <c r="D120" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="121" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C121" s="9"/>
+      <c r="D121" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="122" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C122" s="9"/>
+      <c r="D122" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="117" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C117" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D117" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="118" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C118" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D118" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="119" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C119" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D119" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="120" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C120" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D120" s="3"/>
-    </row>
-    <row r="121" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C121" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D121" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="122" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C122" s="22"/>
-      <c r="D122" s="20" t="s">
-        <v>55</v>
-      </c>
-    </row>
     <row r="123" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C123" s="23"/>
-      <c r="D123" s="21"/>
+      <c r="C123" s="9"/>
+      <c r="D123" s="3" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="124" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C124" s="11"/>
-      <c r="D124" s="19" t="s">
-        <v>72</v>
+      <c r="C124" s="9"/>
+      <c r="D124" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="125" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C125" s="9"/>
       <c r="D125" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="126" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C126" s="9"/>
-      <c r="D126" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="127" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C127" s="9"/>
-      <c r="D127" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="128" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C128" s="9"/>
-      <c r="D128" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="129" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C129" s="9"/>
-      <c r="D129" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="130" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C130" s="9"/>
-      <c r="D130" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="131" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C131" s="9"/>
-      <c r="D131" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="132" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C132" s="9"/>
-      <c r="D132" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="133" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C133" s="9"/>
-      <c r="D133" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="134" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C134" s="9"/>
-      <c r="D134" s="3" t="s">
         <v>64</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="D122:D123"/>
-    <mergeCell ref="C122:C123"/>
+  <mergeCells count="1">
+    <mergeCell ref="D66:D67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
aggiunta bottone di eliminazione pianificazione, corretto barra di ricerca admin, aggiunti requisiti
</commit_message>
<xml_diff>
--- a/Progettazione/Analisi/Requisiti.xlsx
+++ b/Progettazione/Analisi/Requisiti.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MPT\Progettazione\Analisi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MPT\Progettazione\Analisi\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="96">
   <si>
     <t>ID</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Sotto requisiti</t>
   </si>
   <si>
-    <t>Realizzare un sito web per la gestione MPT</t>
-  </si>
-  <si>
     <t>Sito web responsive</t>
   </si>
   <si>
@@ -86,12 +83,6 @@
     <t>I campi devono essere obbligatori</t>
   </si>
   <si>
-    <t>impedire operazioni automatici(robotici)</t>
-  </si>
-  <si>
-    <t>la conferma della registrazione deve avvenire entro 3 giorni</t>
-  </si>
-  <si>
     <t>REQ-004</t>
   </si>
   <si>
@@ -179,15 +170,6 @@
     <t>Permessi</t>
   </si>
   <si>
-    <t>tutti hanno accesso alla pagina login</t>
-  </si>
-  <si>
-    <t>accesso a "Gestione Accessi Docenti" solo a R</t>
-  </si>
-  <si>
-    <t>accesso a "Visione pianificazione… (Responsabile)" solo a R</t>
-  </si>
-  <si>
     <t>La registrazione deve essere confermata da gestore email prima di effettuare il login</t>
   </si>
   <si>
@@ -200,33 +182,6 @@
     <t>C'è un gestore delle email</t>
   </si>
   <si>
-    <t>tutti hanno accesso alla pagina di registrazione</t>
-  </si>
-  <si>
-    <t>tutti hanno accesso alla pagina di password dimenticata</t>
-  </si>
-  <si>
-    <t>accesso a "Menu Principale AIT" a tutti quelli che hanno effettuato il login</t>
-  </si>
-  <si>
-    <t>accesso a "Inserimento ore AIT" solo agli user di tipo docente</t>
-  </si>
-  <si>
-    <t>accesso a "Visione pianificazione… (docente)" solo agli user di tipo docente</t>
-  </si>
-  <si>
-    <t>accesso a "Visione pianificazione completa…" a tutti quelli loggati</t>
-  </si>
-  <si>
-    <t>accesso a "Visioni particolari" a tutti quelli che hanno effettuato il login</t>
-  </si>
-  <si>
-    <t>l'admin ha accesso a tutte le pagine web</t>
-  </si>
-  <si>
-    <t>accesso a "Pianificazione Docenti MPT (Responsabile)" solo a R</t>
-  </si>
-  <si>
     <t>Ha solo accesso alle pagine del responsabile</t>
   </si>
   <si>
@@ -234,6 +189,129 @@
   </si>
   <si>
     <t>Può aggiungere o eliminare dati nel DB(materie,classi,corso,...) tramite il sito web</t>
+  </si>
+  <si>
+    <t>La registrazione è possibile sono con @edu.ti.ch</t>
+  </si>
+  <si>
+    <t>La consegna è il 22.12.2016</t>
+  </si>
+  <si>
+    <t>Realizzare un sito web per la gestione MP</t>
+  </si>
+  <si>
+    <t>Impedire operazioni automatiche (robotici)</t>
+  </si>
+  <si>
+    <t>Quando viene effettuata la registrazione, l'utente ottiene una password momentanea</t>
+  </si>
+  <si>
+    <t>L'utente deve effettuare il login entro 3 giorni dalla conferma della registrazione</t>
+  </si>
+  <si>
+    <t>REQ-008</t>
+  </si>
+  <si>
+    <t>L'admin ha accesso a tutte le pagine web</t>
+  </si>
+  <si>
+    <t>Tutti hanno accesso alla pagina di registrazione</t>
+  </si>
+  <si>
+    <t>Tutti hanno accesso alla pagina di password dimenticata</t>
+  </si>
+  <si>
+    <t>Tutti hanno accesso alla pagina login</t>
+  </si>
+  <si>
+    <t>Accesso a "Gestione Accessi Docenti" solo a R</t>
+  </si>
+  <si>
+    <t>Accesso a "Menu Principale AIT" a tutti quelli che hanno effettuato il login</t>
+  </si>
+  <si>
+    <t>Accesso a "Pianificazione Docenti MPT (Responsabile)" solo a R</t>
+  </si>
+  <si>
+    <t>Accesso a "Inserimento ore AIT" solo agli user di tipo docente</t>
+  </si>
+  <si>
+    <t>Accesso a "Visione pianificazione… (Responsabile)" solo a R</t>
+  </si>
+  <si>
+    <t>Accesso a "Visione pianificazione… (docente)" solo agli user di tipo docente</t>
+  </si>
+  <si>
+    <t>Accesso a "Visione pianificazione completa…" a tutti quelli loggati</t>
+  </si>
+  <si>
+    <t>Accesso a "Visioni particolari" a tutti quelli che hanno effettuato il login</t>
+  </si>
+  <si>
+    <t>Pagina Gestione Accessi Docenti</t>
+  </si>
+  <si>
+    <t>Nel momento della registrazione l'utente deve essere almeno docente</t>
+  </si>
+  <si>
+    <t>Bisogna prevedere una conferma prima della cancellazione di un utente</t>
+  </si>
+  <si>
+    <t>Bisogna poter leggere nome,cognome,email e tipi di ogni docente</t>
+  </si>
+  <si>
+    <t>Nessuno deve potersi autoeliminare tramite il bottone</t>
+  </si>
+  <si>
+    <t>Pagina Pianificazione Docenti MP</t>
+  </si>
+  <si>
+    <t>Bisogna pianificare un minimo di 2 docenti</t>
+  </si>
+  <si>
+    <t>La durata del ciclo cambia in automatico in base al corso</t>
+  </si>
+  <si>
+    <t>Tipo MPT,Classe,Durata e Inizio Ciclo Formativo devono essere dei menu a tendina</t>
+  </si>
+  <si>
+    <t>Il menu a tendina della classe cambia in automatico in base al corso</t>
+  </si>
+  <si>
+    <t>La fine ciclo formativo cambia in base alla durata del corso e inizio del ciclo</t>
+  </si>
+  <si>
+    <t>REQ-012</t>
+  </si>
+  <si>
+    <t>REQ-013</t>
+  </si>
+  <si>
+    <t>Pagina Inserimento ore AIT Docente</t>
+  </si>
+  <si>
+    <t>Accessibile solo ai docenti e all'Amministratore</t>
+  </si>
+  <si>
+    <t>Accessibile solo al Responsabile e all'Amministratore</t>
+  </si>
+  <si>
+    <t>REQ-014</t>
+  </si>
+  <si>
+    <t>Bisogna avere una barra di ricerca per i docenti</t>
+  </si>
+  <si>
+    <t>Bisogna poter inserire le proprie ore di lavoro</t>
+  </si>
+  <si>
+    <t>Bisogna calcolare la percentuale oreDiLavoro/oreTotali*100</t>
+  </si>
+  <si>
+    <t>Bisogna avere un bottone per vedere in dettaglio la pianificazione del docente in lettura</t>
+  </si>
+  <si>
+    <t>Bisogna poter salvare le modifiche tramite un apposito bottone</t>
   </si>
 </sst>
 </file>
@@ -321,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -356,9 +434,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -375,6 +450,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -656,10 +746,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:D125"/>
+  <dimension ref="C1:D176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+    <sheetView tabSelected="1" topLeftCell="A107" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D174" sqref="D174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -683,7 +773,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -719,25 +809,25 @@
     <row r="9" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C9" s="9"/>
       <c r="D9" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C10" s="10"/>
       <c r="D10" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C11" s="10"/>
       <c r="D11" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C12" s="9"/>
       <c r="D12" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -749,7 +839,7 @@
         <v>0</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -757,7 +847,7 @@
         <v>2</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -793,24 +883,26 @@
     <row r="20" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C20" s="10"/>
       <c r="D20" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C21" s="9"/>
       <c r="D21" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C22" s="9"/>
       <c r="D22" s="3" t="s">
-        <v>20</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C23" s="9"/>
-      <c r="D23" s="3"/>
+      <c r="D23" s="3" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="24" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C24" s="9"/>
@@ -822,7 +914,7 @@
         <v>0</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -830,7 +922,7 @@
         <v>2</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -864,606 +956,900 @@
       </c>
     </row>
     <row r="32" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C32" s="10"/>
-      <c r="D32" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="33" spans="3:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C33" s="9"/>
-      <c r="D33" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="34" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C32" s="8"/>
+      <c r="D32" s="19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C33" s="10"/>
+      <c r="D33" s="20"/>
+    </row>
+    <row r="34" spans="3:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C34" s="9"/>
-      <c r="D34" s="3" t="s">
-        <v>55</v>
+      <c r="D34" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C35" s="9"/>
-      <c r="D35" s="3"/>
-    </row>
-    <row r="36" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+      <c r="D35" s="19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C36" s="9"/>
+      <c r="D36" s="20"/>
+    </row>
     <row r="37" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C37" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="38" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C38" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
+      <c r="C37" s="9"/>
+      <c r="D37" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="39" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C39" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D39" s="3">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="40" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C40" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="41" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C41" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D41" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="D41" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="42" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C42" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C43" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" s="3"/>
+    </row>
+    <row r="44" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C44" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="D44" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C43" s="10"/>
-      <c r="D43" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="44" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C44" s="10"/>
-      <c r="D44" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
     <row r="45" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C45" s="12"/>
-      <c r="D45" s="13"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="46" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C46" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D46" s="7" t="s">
-        <v>22</v>
+      <c r="C46" s="10"/>
+      <c r="D46" s="4" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="47" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C47" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="C47" s="12"/>
+      <c r="D47" s="13"/>
     </row>
     <row r="48" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C48" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D48" s="3">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="49" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C49" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="50" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C50" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D50" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="D50" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="51" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C51" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C52" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" s="3"/>
+    </row>
+    <row r="53" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C53" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="D53" s="7" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="52" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C52" s="9"/>
-      <c r="D52" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="53" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C53" s="9"/>
-      <c r="D53" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="54" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C54" s="9"/>
       <c r="D54" s="3" t="s">
-        <v>57</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C55" s="9"/>
       <c r="D55" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="56" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="56" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C56" s="9"/>
+      <c r="D56" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
     <row r="57" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C57" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D57" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="58" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C58" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
+      <c r="C57" s="9"/>
+      <c r="D57" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="58" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="59" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C59" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D59" s="3">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="60" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C60" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D60" s="6" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="61" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C61" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D61" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="D61" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="62" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C62" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C63" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D63" s="3"/>
+    </row>
+    <row r="64" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C64" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D62" s="7" t="s">
+      <c r="D64" s="7" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="63" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C63" s="9"/>
-      <c r="D63" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="64" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C64" s="10"/>
-      <c r="D64" s="4" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="65" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C65" s="9"/>
       <c r="D65" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="66" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C66" s="9"/>
-      <c r="D66" s="20" t="s">
-        <v>69</v>
+      <c r="C66" s="10"/>
+      <c r="D66" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="67" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C67" s="9"/>
-      <c r="D67" s="21"/>
+      <c r="D67" s="3" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="68" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C68" s="9"/>
-      <c r="D68" s="3" t="s">
-        <v>46</v>
+      <c r="D68" s="19" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="69" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C69" s="9"/>
-      <c r="D69" s="3" t="s">
-        <v>47</v>
-      </c>
+      <c r="D69" s="20"/>
     </row>
     <row r="70" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C70" s="9"/>
       <c r="D70" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="71" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C71" s="1"/>
+      <c r="C71" s="9"/>
+      <c r="D71" s="3" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="72" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C72" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D72" s="7" t="s">
-        <v>27</v>
+      <c r="C72" s="9"/>
+      <c r="D72" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="73" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C73" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="C73" s="1"/>
     </row>
     <row r="74" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C74" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D74" s="3">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D74" s="7" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="75" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C75" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D75" s="6" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="76" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C76" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D76" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="D76" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="77" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C77" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C78" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D78" s="3"/>
+    </row>
+    <row r="79" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C79" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D77" s="7" t="s">
+      <c r="D79" s="7" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="78" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C78" s="9"/>
-      <c r="D78" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="79" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C79" s="9"/>
-      <c r="D79" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="80" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C80" s="9"/>
       <c r="D80" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="81" spans="3:4" s="18" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C81" s="16"/>
-      <c r="D81" s="17" t="s">
-        <v>44</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="81" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C81" s="9"/>
+      <c r="D81" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="82" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C82" s="9"/>
       <c r="D82" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="83" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C83" s="9"/>
-      <c r="D83" s="3" t="s">
-        <v>67</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="83" spans="3:4" s="17" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C83" s="15"/>
+      <c r="D83" s="16" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="84" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C84" s="9"/>
       <c r="D84" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="85" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C85" s="10"/>
-      <c r="D85" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="86" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="87" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C87" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D87" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="88" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C88" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D88" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
+      <c r="C85" s="9"/>
+      <c r="D85" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="86" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C86" s="9"/>
+      <c r="D86" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="87" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C87" s="10"/>
+      <c r="D87" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="88" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="89" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C89" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D89" s="3">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D89" s="7" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="90" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C90" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D90" s="6" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="91" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C91" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D91" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="D91" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="92" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C92" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D92" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="93" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C93" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D93" s="3"/>
+    </row>
+    <row r="94" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C94" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D92" s="7" t="s">
+      <c r="D94" s="7" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="93" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C93" s="10"/>
-      <c r="D93" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="94" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C94" s="10"/>
-      <c r="D94" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="95" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C95" s="10"/>
-      <c r="D95" s="3" t="s">
-        <v>68</v>
+      <c r="D95" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="96" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C96" s="10"/>
       <c r="D96" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="97" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C97" s="9"/>
+      <c r="C97" s="10"/>
       <c r="D97" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="98" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="98" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C98" s="10"/>
+      <c r="D98" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
     <row r="99" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C99" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D99" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="100" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C100" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D100" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
+      <c r="C99" s="9"/>
+      <c r="D99" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="100" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="101" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C101" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D101" s="3">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D101" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="102" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C102" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D102" s="6" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="103" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C103" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D103" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="D103" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="104" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C104" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D104" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="105" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C105" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D105" s="3"/>
+    </row>
+    <row r="106" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C106" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D104" s="7" t="s">
+      <c r="D106" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="105" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C105" s="9"/>
-      <c r="D105" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="106" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C106" s="9"/>
-      <c r="D106" s="3"/>
-    </row>
-    <row r="107" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="107" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C107" s="9"/>
+      <c r="D107" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
     <row r="108" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C108" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D108" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="109" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C109" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D109" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
+      <c r="C108" s="9"/>
+      <c r="D108" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="109" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="110" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C110" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D110" s="3">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D110" s="7" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="111" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C111" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D111" s="6" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="112" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C112" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D112" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="D112" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="113" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C113" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D113" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="114" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C114" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D114" s="3"/>
+    </row>
+    <row r="115" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C115" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D113" s="7" t="s">
+      <c r="D115" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="114" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C114" s="19"/>
-      <c r="D114" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="115" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C115" s="11"/>
-      <c r="D115" s="14" t="s">
-        <v>58</v>
-      </c>
-    </row>
     <row r="116" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C116" s="15"/>
-      <c r="D116" s="14" t="s">
-        <v>59</v>
+      <c r="C116" s="18"/>
+      <c r="D116" s="21" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="117" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C117" s="9"/>
-      <c r="D117" s="3" t="s">
-        <v>51</v>
+      <c r="C117" s="11"/>
+      <c r="D117" s="22" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="118" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C118" s="9"/>
-      <c r="D118" s="3" t="s">
-        <v>52</v>
+      <c r="C118" s="14"/>
+      <c r="D118" s="22" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="119" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C119" s="9"/>
-      <c r="D119" s="3" t="s">
-        <v>60</v>
+      <c r="D119" s="16" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="120" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C120" s="9"/>
-      <c r="D120" s="3" t="s">
+      <c r="D120" s="16" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="121" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C121" s="9"/>
-      <c r="D121" s="3" t="s">
-        <v>61</v>
+      <c r="D121" s="16" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="122" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C122" s="9"/>
-      <c r="D122" s="3" t="s">
-        <v>53</v>
+      <c r="D122" s="16" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="123" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C123" s="9"/>
-      <c r="D123" s="3" t="s">
-        <v>62</v>
+      <c r="D123" s="16" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="124" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C124" s="9"/>
-      <c r="D124" s="3" t="s">
-        <v>63</v>
+      <c r="D124" s="16" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="125" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C125" s="9"/>
-      <c r="D125" s="3" t="s">
-        <v>64</v>
-      </c>
+      <c r="D125" s="16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="126" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C126" s="9"/>
+      <c r="D126" s="16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="127" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C127" s="9"/>
+      <c r="D127" s="16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="128" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="129" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C129" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D129" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="130" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C130" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D130" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="131" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C131" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D131" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C132" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D132" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="133" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C133" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D133" s="3"/>
+    </row>
+    <row r="134" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C134" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D134" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="135" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C135" s="10"/>
+      <c r="D135" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="136" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C136" s="10"/>
+      <c r="D136" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="137" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C137" s="10"/>
+      <c r="D137" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="138" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C138" s="10"/>
+      <c r="D138" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="139" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C139" s="9"/>
+      <c r="D139" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="140" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C140" s="9"/>
+      <c r="D140" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="141" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="142" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C142" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D142" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="143" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C143" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D143" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="144" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C144" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D144" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C145" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D145" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="146" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C146" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D146" s="3"/>
+    </row>
+    <row r="147" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C147" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D147" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="148" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C148" s="10"/>
+      <c r="D148" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="149" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C149" s="10"/>
+      <c r="D149" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="150" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C150" s="10"/>
+      <c r="D150" s="19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="151" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C151" s="10"/>
+      <c r="D151" s="20"/>
+    </row>
+    <row r="152" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C152" s="10"/>
+      <c r="D152" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="153" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C153" s="9"/>
+      <c r="D153" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="154" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C154" s="9"/>
+      <c r="D154" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="155" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="156" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C156" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D156" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="157" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C157" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D157" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="158" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C158" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D158" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C159" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D159" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="160" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C160" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D160" s="3"/>
+    </row>
+    <row r="161" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C161" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D161" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="162" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C162" s="10"/>
+      <c r="D162" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="163" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C163" s="10"/>
+      <c r="D163" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="164" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C164" s="10"/>
+      <c r="D164" s="23" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="165" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C165" s="10"/>
+      <c r="D165" s="24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="166" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C166" s="10"/>
+      <c r="D166" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="167" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C167" s="9"/>
+      <c r="D167" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="168" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C168" s="9"/>
+      <c r="D168" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="169" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C169" s="9"/>
+      <c r="D169" s="19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="170" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C170" s="9"/>
+      <c r="D170" s="20"/>
+    </row>
+    <row r="171" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C171" s="9"/>
+      <c r="D171" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="176" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D176" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D66:D67"/>
+  <mergeCells count="5">
+    <mergeCell ref="D169:D170"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="D150:D151"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
diari,doc, aggiunta commenti file
</commit_message>
<xml_diff>
--- a/Progettazione/Analisi/Requisiti.xlsx
+++ b/Progettazione/Analisi/Requisiti.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MPT\Progettazione\Analisi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MPT\Progettazione\Analisi\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,6 +15,7 @@
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="119">
   <si>
     <t>ID</t>
   </si>
@@ -251,9 +252,6 @@
     <t>Pagina Gestione Accessi Docenti</t>
   </si>
   <si>
-    <t>Nel momento della registrazione l'utente deve essere almeno docente</t>
-  </si>
-  <si>
     <t>Bisogna prevedere una conferma prima della cancellazione di un utente</t>
   </si>
   <si>
@@ -272,9 +270,6 @@
     <t>La durata del ciclo cambia in automatico in base al corso</t>
   </si>
   <si>
-    <t>Tipo MPT,Classe,Durata e Inizio Ciclo Formativo devono essere dei menu a tendina</t>
-  </si>
-  <si>
     <t>Il menu a tendina della classe cambia in automatico in base al corso</t>
   </si>
   <si>
@@ -312,6 +307,81 @@
   </si>
   <si>
     <t>Bisogna poter salvare le modifiche tramite un apposito bottone</t>
+  </si>
+  <si>
+    <t>REQ-015</t>
+  </si>
+  <si>
+    <t>Pagina Visione Pianificazione Docenti MP (Responsabile)</t>
+  </si>
+  <si>
+    <t>Accessibile solo ai responsabili e all'Amministratore</t>
+  </si>
+  <si>
+    <t>Bisogna avere una barra di ricerca per trovare le pianificazioni</t>
+  </si>
+  <si>
+    <t>Bisogna poter vedere la percentuale di lavoro dei docenti in lettura</t>
+  </si>
+  <si>
+    <t>Bisogna avere un bottone per l'eliminazione della pianificazione tramite una conferma</t>
+  </si>
+  <si>
+    <t>Pagina Visione Pianificazione Docenti MP (Docente)</t>
+  </si>
+  <si>
+    <t>REQ-016</t>
+  </si>
+  <si>
+    <t>Bisogna poter vedere tutte le informazioni delle pianificazioni</t>
+  </si>
+  <si>
+    <t>REQ-017</t>
+  </si>
+  <si>
+    <t>Pagina visioni particolari</t>
+  </si>
+  <si>
+    <t>Pagina Visione pianificazione completa docenti MP</t>
+  </si>
+  <si>
+    <t>Bisogna poter vedere tutte le pianificazioni di tutti i docenti</t>
+  </si>
+  <si>
+    <t>Bisogna avere una barra di ricerca per cercare le pianificazioni</t>
+  </si>
+  <si>
+    <t>Bisogna avere dei checkbox che quando checkati visualizzano le rispettive colonne</t>
+  </si>
+  <si>
+    <t>Bisogna poter creare un pdf per il salvataggio della tabella filtrata</t>
+  </si>
+  <si>
+    <t>Bisogna poter stampare il pdf</t>
+  </si>
+  <si>
+    <t>REQ-011</t>
+  </si>
+  <si>
+    <t>Nel momento della registrazione l'utente deve essere di tipo docente</t>
+  </si>
+  <si>
+    <t>Tipo MP,Classe,Durata e Inizio Ciclo Formativo devono essere dei menu a tendina</t>
+  </si>
+  <si>
+    <t>Bisogna avere una barra di ricerca per le pianificazioni</t>
+  </si>
+  <si>
+    <t>Bisogna poter vedere le proprie percentuali di lavoro in lettura</t>
+  </si>
+  <si>
+    <t>Bisogna avere un bottone per vedere in dettaglio la propria pianificazione in lettura</t>
+  </si>
+  <si>
+    <t>Bisogna poter vedere tutte le informazioni della pianificazione creata insieme a tutte le parti dei docenti coinvolti in lettura</t>
+  </si>
+  <si>
+    <t>Accessibile a tutte le persone loggate</t>
   </si>
 </sst>
 </file>
@@ -346,7 +416,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -393,6 +463,17 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -445,26 +526,26 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -746,10 +827,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:D176"/>
+  <dimension ref="C1:D219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D174" sqref="D174"/>
+    <sheetView tabSelected="1" topLeftCell="A209" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D213" sqref="D213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -957,13 +1038,13 @@
     </row>
     <row r="32" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C32" s="8"/>
-      <c r="D32" s="19" t="s">
+      <c r="D32" s="23" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="33" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C33" s="10"/>
-      <c r="D33" s="20"/>
+      <c r="D33" s="24"/>
     </row>
     <row r="34" spans="3:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C34" s="9"/>
@@ -973,13 +1054,13 @@
     </row>
     <row r="35" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C35" s="9"/>
-      <c r="D35" s="19" t="s">
+      <c r="D35" s="23" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="36" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C36" s="9"/>
-      <c r="D36" s="20"/>
+      <c r="D36" s="24"/>
     </row>
     <row r="37" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C37" s="9"/>
@@ -1187,13 +1268,13 @@
     </row>
     <row r="68" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C68" s="9"/>
-      <c r="D68" s="19" t="s">
+      <c r="D68" s="23" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="69" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C69" s="9"/>
-      <c r="D69" s="20"/>
+      <c r="D69" s="24"/>
     </row>
     <row r="70" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C70" s="9"/>
@@ -1495,19 +1576,19 @@
     </row>
     <row r="116" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C116" s="18"/>
-      <c r="D116" s="21" t="s">
+      <c r="D116" s="19" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="117" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C117" s="11"/>
-      <c r="D117" s="22" t="s">
+      <c r="D117" s="20" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="118" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C118" s="14"/>
-      <c r="D118" s="22" t="s">
+      <c r="D118" s="20" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1571,7 +1652,7 @@
         <v>0</v>
       </c>
       <c r="D129" s="7" t="s">
-        <v>85</v>
+        <v>111</v>
       </c>
     </row>
     <row r="130" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1615,37 +1696,37 @@
     <row r="135" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C135" s="10"/>
       <c r="D135" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="136" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C136" s="10"/>
       <c r="D136" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="137" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C137" s="10"/>
       <c r="D137" s="3" t="s">
-        <v>75</v>
+        <v>112</v>
       </c>
     </row>
     <row r="138" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C138" s="10"/>
       <c r="D138" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="139" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C139" s="9"/>
       <c r="D139" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="140" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C140" s="9"/>
       <c r="D140" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="141" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1654,7 +1735,7 @@
         <v>0</v>
       </c>
       <c r="D142" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="143" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1662,7 +1743,7 @@
         <v>2</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="144" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1698,41 +1779,41 @@
     <row r="148" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C148" s="10"/>
       <c r="D148" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="149" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C149" s="10"/>
       <c r="D149" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="150" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C150" s="10"/>
-      <c r="D150" s="19" t="s">
-        <v>82</v>
+      <c r="D150" s="23" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="151" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C151" s="10"/>
-      <c r="D151" s="20"/>
+      <c r="D151" s="24"/>
     </row>
     <row r="152" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C152" s="10"/>
       <c r="D152" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="153" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C153" s="9"/>
       <c r="D153" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="154" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C154" s="9"/>
       <c r="D154" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="155" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1741,7 +1822,7 @@
         <v>0</v>
       </c>
       <c r="D156" s="7" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="157" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1749,7 +1830,7 @@
         <v>2</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="158" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1785,67 +1866,367 @@
     <row r="162" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C162" s="10"/>
       <c r="D162" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="163" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C163" s="10"/>
       <c r="D163" s="3" t="s">
-        <v>91</v>
+        <v>114</v>
       </c>
     </row>
     <row r="164" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C164" s="10"/>
-      <c r="D164" s="23" t="s">
-        <v>92</v>
+      <c r="D164" s="22" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="165" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C165" s="10"/>
-      <c r="D165" s="24" t="s">
-        <v>93</v>
+      <c r="D165" s="21" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="166" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C166" s="10"/>
-      <c r="D166" s="3" t="s">
-        <v>81</v>
+      <c r="C166" s="9"/>
+      <c r="D166" s="23" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="167" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C167" s="9"/>
-      <c r="D167" s="3" t="s">
-        <v>83</v>
-      </c>
+      <c r="D167" s="24"/>
     </row>
     <row r="168" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C168" s="9"/>
       <c r="D168" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="169" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C169" s="9"/>
-      <c r="D169" s="19" t="s">
-        <v>94</v>
-      </c>
-    </row>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="169" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="170" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C170" s="9"/>
-      <c r="D170" s="20"/>
+      <c r="C170" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D170" s="7" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="171" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C171" s="9"/>
+      <c r="C171" s="8" t="s">
+        <v>2</v>
+      </c>
       <c r="D171" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="176" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="D176" s="25"/>
+    <row r="172" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C172" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D172" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C173" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D173" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="174" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C174" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D174" s="3"/>
+    </row>
+    <row r="175" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C175" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D175" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="176" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C176" s="10"/>
+      <c r="D176" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="177" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C177" s="10"/>
+      <c r="D177" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="178" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C178" s="10"/>
+      <c r="D178" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="179" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C179" s="10"/>
+      <c r="D179" s="22" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="180" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C180" s="10"/>
+      <c r="D180" s="23" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="181" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C181" s="9"/>
+      <c r="D181" s="24"/>
+    </row>
+    <row r="182" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C182" s="9"/>
+      <c r="D182" s="23" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="183" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C183" s="9"/>
+      <c r="D183" s="24"/>
+    </row>
+    <row r="184" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="185" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C185" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D185" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="186" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C186" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D186" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="187" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C187" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D187" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C188" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D188" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="189" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C189" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D189" s="3"/>
+    </row>
+    <row r="190" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C190" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D190" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="191" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C191" s="10"/>
+      <c r="D191" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="192" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C192" s="10"/>
+      <c r="D192" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="193" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C193" s="10"/>
+      <c r="D193" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="194" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C194" s="10"/>
+      <c r="D194" s="22" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="195" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C195" s="9"/>
+      <c r="D195" s="23" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="196" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C196" s="9"/>
+      <c r="D196" s="24"/>
+    </row>
+    <row r="197" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="198" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C198" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D198" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="199" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C199" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D199" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="200" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C200" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D200" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C201" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D201" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="202" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C202" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D202" s="3"/>
+    </row>
+    <row r="203" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C203" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D203" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="204" spans="3:4" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C204" s="10"/>
+      <c r="D204" s="23" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="205" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C205" s="10"/>
+      <c r="D205" s="24"/>
+    </row>
+    <row r="206" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="207" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C207" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D207" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="208" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C208" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D208" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="209" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C209" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D209" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C210" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D210" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="211" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C211" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D211" s="3"/>
+    </row>
+    <row r="212" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C212" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D212" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="213" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C213" s="10"/>
+      <c r="D213" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="214" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C214" s="10"/>
+      <c r="D214" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="215" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C215" s="10"/>
+      <c r="D215" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="216" spans="3:4" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C216" s="10"/>
+      <c r="D216" s="23" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="217" spans="3:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C217" s="9"/>
+      <c r="D217" s="25"/>
+    </row>
+    <row r="218" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C218" s="9"/>
+      <c r="D218" s="22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="219" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C219" s="9"/>
+      <c r="D219" s="3" t="s">
+        <v>110</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="D169:D170"/>
+  <mergeCells count="10">
+    <mergeCell ref="D204:D205"/>
+    <mergeCell ref="D216:D217"/>
+    <mergeCell ref="D182:D183"/>
+    <mergeCell ref="D180:D181"/>
+    <mergeCell ref="D195:D196"/>
+    <mergeCell ref="D166:D167"/>
     <mergeCell ref="D68:D69"/>
     <mergeCell ref="D35:D36"/>
     <mergeCell ref="D32:D33"/>

</xml_diff>